<commit_message>
code and files for consistency and form along with team detailsand aslo final dataset
</commit_message>
<xml_diff>
--- a/cleaned all season/allrounderset_smat.xlsx
+++ b/cleaned all season/allrounderset_smat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/Dataset_Final/all seasons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/cricket-squad-selection/cleaned all season/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30BC5F2-09CE-A144-8FF4-34B59C62CD6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC9DFC6-9083-7A45-ACEE-C2BB651C26E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1840" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Player</t>
   </si>
@@ -155,13 +155,31 @@
   </si>
   <si>
     <t>L Manvanth Kumar</t>
+  </si>
+  <si>
+    <t>J Overton</t>
+  </si>
+  <si>
+    <t>2023-2025</t>
+  </si>
+  <si>
+    <t>AM Hardie</t>
+  </si>
+  <si>
+    <t>2019-2025</t>
+  </si>
+  <si>
+    <t>PHKD Mendis</t>
+  </si>
+  <si>
+    <t>2020-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +192,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,13 +236,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,983 +552,1243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2:AB11"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>46</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>36</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>450</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>49</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <v>17.3</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
         <v>335</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>134.32</v>
       </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
         <v>2</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="3">
         <v>31</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="3">
         <v>24</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="3">
         <v>46</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="3">
         <v>44</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="3">
         <v>145.5</v>
       </c>
-      <c r="S2" s="2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2">
+      <c r="S2" s="3">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3">
         <v>1037</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="3">
         <v>44</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="3">
         <v>23.56</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="3">
         <v>7.11</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="3">
         <v>19.8</v>
       </c>
-      <c r="Y2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="2" t="s">
+      <c r="Y2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
         <v>21</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>13</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>21</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <v>15</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="3">
         <v>140</v>
       </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
         <v>2</v>
       </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
         <v>3</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="3">
         <v>3</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="3">
         <v>7</v>
       </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2">
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3">
         <v>68</v>
       </c>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2">
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
         <v>100</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3" s="3">
         <v>9.7100000000000009</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3" s="3">
         <v>100</v>
       </c>
-      <c r="Y3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="2" t="s">
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>28</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>15</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>187</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>41</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>15.58</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <v>141</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="3">
         <v>132.62</v>
       </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
         <v>9</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="3">
         <v>12</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="3">
         <v>28</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="3">
         <v>22</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="3">
         <v>50</v>
       </c>
-      <c r="S4" s="2">
-        <v>0</v>
-      </c>
-      <c r="T4" s="2">
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
         <v>433</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="3">
         <v>18</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="3">
         <v>24.05</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4" s="3">
         <v>8.66</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="3">
         <v>16.600000000000001</v>
       </c>
-      <c r="Y4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="2" t="s">
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>22</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>21</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>4</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>431</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>100</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>25.35</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>351</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3">
         <v>122.79</v>
       </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
         <v>35</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="3">
         <v>14</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="3">
         <v>22</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="3">
         <v>18</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="3">
         <v>45</v>
       </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2">
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="3">
         <v>282</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="3">
         <v>14</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="3">
         <v>20.14</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5" s="3">
         <v>6.26</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5" s="3">
         <v>19.2</v>
       </c>
-      <c r="Y5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="2" t="s">
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>18</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>18</v>
       </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
         <v>573</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>102</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>33.700000000000003</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <v>344</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <v>166.56</v>
       </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
         <v>3</v>
       </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
         <v>54</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="3">
         <v>36</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="3">
         <v>18</v>
       </c>
-      <c r="Q6" s="2">
-        <v>1</v>
-      </c>
-      <c r="R6" s="2">
-        <v>1</v>
-      </c>
-      <c r="S6" s="2">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2">
+      <c r="Q6" s="3">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3">
+        <v>1</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3">
         <v>2</v>
       </c>
-      <c r="U6" s="2">
-        <v>1</v>
-      </c>
-      <c r="V6" s="2">
+      <c r="U6" s="3">
+        <v>1</v>
+      </c>
+      <c r="V6" s="3">
         <v>2</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6" s="3">
         <v>2</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6" s="3">
         <v>6</v>
       </c>
-      <c r="Y6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2" t="s">
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB6" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>6</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>30</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>13</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>7.5</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <v>20</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="3">
         <v>150</v>
       </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
         <v>4</v>
       </c>
-      <c r="O7" s="2">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2">
+      <c r="O7" s="3">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3">
         <v>6</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="3">
         <v>6</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="3">
         <v>16</v>
       </c>
-      <c r="S7" s="2">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2">
+      <c r="S7" s="3">
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
         <v>174</v>
       </c>
-      <c r="U7" s="2">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2">
+      <c r="U7" s="3">
+        <v>1</v>
+      </c>
+      <c r="V7" s="3">
         <v>174</v>
       </c>
-      <c r="W7" s="2">
+      <c r="W7" s="3">
         <v>10.87</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7" s="3">
         <v>96</v>
       </c>
-      <c r="Y7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="2" t="s">
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AB7" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>9</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>9</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>131</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>36</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>43.66</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <v>52</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="3">
         <v>251.92</v>
       </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
         <v>7</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="3">
         <v>13</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="3">
         <v>9</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="3">
         <v>9</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="3">
         <v>19.5</v>
       </c>
-      <c r="S8" s="2">
-        <v>0</v>
-      </c>
-      <c r="T8" s="2">
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3">
         <v>184</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="3">
         <v>8</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8" s="3">
         <v>23</v>
       </c>
-      <c r="W8" s="2">
+      <c r="W8" s="3">
         <v>9.27</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8" s="3">
         <v>14.8</v>
       </c>
-      <c r="Y8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="2" t="s">
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AB8" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>4</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
         <v>46</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>23</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>11.5</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <v>53</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="3">
         <v>86.79</v>
       </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
         <v>4</v>
       </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2">
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3">
         <v>8</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="3">
         <v>8</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="3">
         <v>31</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="3">
         <v>2</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="3">
         <v>186</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="3">
         <v>12</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9" s="3">
         <v>15.5</v>
       </c>
-      <c r="W9" s="2">
+      <c r="W9" s="3">
         <v>6</v>
       </c>
-      <c r="X9" s="2">
+      <c r="X9" s="3">
         <v>15.5</v>
       </c>
-      <c r="Y9" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="2" t="s">
+      <c r="Y9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AB9" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>7</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
         <v>64</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <v>27</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>16</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <v>41</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="3">
         <v>156.09</v>
       </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
         <v>7</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="3">
         <v>3</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="3">
         <v>7</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q10" s="3">
         <v>7</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="3">
         <v>24</v>
       </c>
-      <c r="S10" s="2">
-        <v>0</v>
-      </c>
-      <c r="T10" s="2">
+      <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="T10" s="3">
         <v>171</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10" s="3">
         <v>8</v>
       </c>
-      <c r="V10" s="2">
+      <c r="V10" s="3">
         <v>21.37</v>
       </c>
-      <c r="W10" s="2">
+      <c r="W10" s="3">
         <v>7.12</v>
       </c>
-      <c r="X10" s="2">
+      <c r="X10" s="3">
         <v>18</v>
       </c>
-      <c r="Y10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="2" t="s">
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AB10" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>15</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>11</v>
       </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
         <v>478</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <v>123</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <v>47.8</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <v>311</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="3">
         <v>153.69</v>
       </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
         <v>3</v>
       </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
         <v>45</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="3">
         <v>27</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="3">
         <v>15</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="3">
         <v>8</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="3">
         <v>22</v>
       </c>
-      <c r="S11" s="2">
-        <v>0</v>
-      </c>
-      <c r="T11" s="2">
+      <c r="S11" s="3">
+        <v>0</v>
+      </c>
+      <c r="T11" s="3">
         <v>131</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="3">
         <v>8</v>
       </c>
-      <c r="V11" s="2">
+      <c r="V11" s="3">
         <v>16.37</v>
       </c>
-      <c r="W11" s="2">
+      <c r="W11" s="3">
         <v>5.95</v>
       </c>
-      <c r="X11" s="2">
+      <c r="X11" s="3">
         <v>16.5</v>
       </c>
-      <c r="Y11" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="2" t="s">
+      <c r="Y11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="AB11" s="3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="4">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4">
+        <v>276</v>
+      </c>
+      <c r="G12" s="4">
+        <v>45</v>
+      </c>
+      <c r="H12" s="4">
+        <v>69</v>
+      </c>
+      <c r="I12" s="4">
+        <v>183</v>
+      </c>
+      <c r="J12" s="4">
+        <v>150.81</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>16</v>
+      </c>
+      <c r="O12" s="4">
+        <v>14</v>
+      </c>
+      <c r="P12" s="4">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>18</v>
+      </c>
+      <c r="R12" s="4">
+        <v>66</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
+        <v>582</v>
+      </c>
+      <c r="U12" s="4">
+        <v>27</v>
+      </c>
+      <c r="V12" s="4">
+        <v>21.55</v>
+      </c>
+      <c r="W12" s="4">
+        <v>8.81</v>
+      </c>
+      <c r="X12" s="4">
+        <v>14.6</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB12" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="4">
+        <v>61</v>
+      </c>
+      <c r="D13" s="4">
+        <v>51</v>
+      </c>
+      <c r="E13" s="4">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1160</v>
+      </c>
+      <c r="G13" s="4">
+        <v>90</v>
+      </c>
+      <c r="H13" s="4">
+        <v>28.29</v>
+      </c>
+      <c r="I13" s="4">
+        <v>891</v>
+      </c>
+      <c r="J13" s="4">
+        <v>130.19</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>6</v>
+      </c>
+      <c r="M13" s="4">
+        <v>3</v>
+      </c>
+      <c r="N13" s="4">
+        <v>82</v>
+      </c>
+      <c r="O13" s="4">
+        <v>46</v>
+      </c>
+      <c r="P13" s="4">
+        <v>61</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>34</v>
+      </c>
+      <c r="R13" s="4">
+        <v>86.1</v>
+      </c>
+      <c r="S13" s="4">
+        <v>0</v>
+      </c>
+      <c r="T13" s="4">
+        <v>713</v>
+      </c>
+      <c r="U13" s="4">
+        <v>26</v>
+      </c>
+      <c r="V13" s="4">
+        <v>27.42</v>
+      </c>
+      <c r="W13" s="4">
+        <v>8.27</v>
+      </c>
+      <c r="X13" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="4">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4">
+        <v>782</v>
+      </c>
+      <c r="G14" s="4">
+        <v>65</v>
+      </c>
+      <c r="H14" s="4">
+        <v>25.22</v>
+      </c>
+      <c r="I14" s="4">
+        <v>636</v>
+      </c>
+      <c r="J14" s="4">
+        <v>122.95</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>5</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>72</v>
+      </c>
+      <c r="O14" s="4">
+        <v>22</v>
+      </c>
+      <c r="P14" s="4">
+        <v>39</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>25</v>
+      </c>
+      <c r="R14" s="4">
+        <v>55</v>
+      </c>
+      <c r="S14" s="4">
+        <v>0</v>
+      </c>
+      <c r="T14" s="4">
+        <v>487</v>
+      </c>
+      <c r="U14" s="4">
+        <v>8</v>
+      </c>
+      <c r="V14" s="4">
+        <v>60.87</v>
+      </c>
+      <c r="W14" s="4">
+        <v>8.85</v>
+      </c>
+      <c r="X14" s="4">
+        <v>41.2</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>